<commit_message>
Added clicks and typings.
</commit_message>
<xml_diff>
--- a/Data/Senaryo 5-Uygulama Kapsam Listesi.xlsx
+++ b/Data/Senaryo 5-Uygulama Kapsam Listesi.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TR995530\Desktop\ITGC-Kontroller\Aura Otomasyon\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TR997437\Desktop\RAS Otomasyon\IT05\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{69EF1791-7AA3-48E4-8B0E-D93AB3652A44}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1669C09-37EA-44A2-A2BC-13D6861B443A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{14B32263-5150-44CF-821E-F92A842F3AFF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{14B32263-5150-44CF-821E-F92A842F3AFF}"/>
   </bookViews>
   <sheets>
     <sheet name="2018-Uygulama-Sistem Özet" sheetId="1" r:id="rId1"/>
@@ -31,32 +31,17 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="21">
-  <si>
-    <t>UC4</t>
-  </si>
-  <si>
-    <t>SAS</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="23">
   <si>
     <t>Parola koruması, Firewall</t>
   </si>
   <si>
-    <t>Mobil Bankacılık</t>
-  </si>
-  <si>
     <t>Fiziksel</t>
   </si>
   <si>
     <t>Microsoft Windows Server 2008 R2</t>
   </si>
   <si>
-    <t>Business Object</t>
-  </si>
-  <si>
-    <t>ATM</t>
-  </si>
-  <si>
     <t>Güvenlik Önlemleri</t>
   </si>
   <si>
@@ -87,13 +72,34 @@
     <t>İstanbul</t>
   </si>
   <si>
-    <t>İnternet Bankacılığı</t>
-  </si>
-  <si>
-    <t>Çağrı Merkezi</t>
-  </si>
-  <si>
     <t>İzmir</t>
+  </si>
+  <si>
+    <t>Application Type Deneme</t>
+  </si>
+  <si>
+    <t>Packaged - Hosted</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>G</t>
   </si>
 </sst>
 </file>
@@ -162,7 +168,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -222,11 +228,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -247,6 +262,12 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -563,229 +584,256 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5A8F6F0-AAFF-46A1-824C-83A9FB192D93}">
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="17.7265625" customWidth="1"/>
-    <col min="3" max="3" width="21.453125" customWidth="1"/>
-    <col min="4" max="4" width="17.7265625" customWidth="1"/>
-    <col min="5" max="5" width="23.08984375" customWidth="1"/>
-    <col min="6" max="7" width="17.7265625" customWidth="1"/>
-    <col min="8" max="8" width="19.1796875" customWidth="1"/>
+    <col min="1" max="2" width="17.7109375" customWidth="1"/>
+    <col min="3" max="3" width="21.42578125" customWidth="1"/>
+    <col min="4" max="4" width="17.7109375" customWidth="1"/>
+    <col min="5" max="5" width="23.140625" customWidth="1"/>
+    <col min="6" max="7" width="17.7109375" customWidth="1"/>
+    <col min="8" max="8" width="19.140625" customWidth="1"/>
+    <col min="9" max="9" width="19.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="26.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="I2" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C1" s="6" t="s">
+    </row>
+    <row r="3" spans="1:9" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="H3" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="I3" s="9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F4" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="G4" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="I4" s="9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="H1" s="6" t="s">
-        <v>8</v>
+      <c r="C5" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="I5" s="9" t="s">
+        <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="26.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G2" s="4" t="s">
+    <row r="6" spans="1:9" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="H2" s="4" t="s">
-        <v>2</v>
+      <c r="B6" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="I6" s="9" t="s">
+        <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="26.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>2</v>
+    <row r="7" spans="1:9" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="I7" s="9" t="s">
+        <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="26.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>2</v>
+    <row r="8" spans="1:9" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="I8" s="9" t="s">
+        <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="26.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="26.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="26.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="H7" s="4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="26.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G8" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="H8" s="4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added if same name exists logic.
</commit_message>
<xml_diff>
--- a/Data/Senaryo 5-Uygulama Kapsam Listesi.xlsx
+++ b/Data/Senaryo 5-Uygulama Kapsam Listesi.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TR997437\Desktop\RAS Otomasyon\IT05\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1669C09-37EA-44A2-A2BC-13D6861B443A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AA9CDA6-7645-48B5-BF1E-692AFCE8C9D9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{14B32263-5150-44CF-821E-F92A842F3AFF}"/>
   </bookViews>
@@ -81,25 +81,25 @@
     <t>Packaged - Hosted</t>
   </si>
   <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>B</t>
-  </si>
-  <si>
-    <t>C</t>
-  </si>
-  <si>
-    <t>D</t>
-  </si>
-  <si>
-    <t>E</t>
-  </si>
-  <si>
-    <t>F</t>
-  </si>
-  <si>
-    <t>G</t>
+    <t>AAAA</t>
+  </si>
+  <si>
+    <t>BBBB</t>
+  </si>
+  <si>
+    <t>CCCC</t>
+  </si>
+  <si>
+    <t>DDDD</t>
+  </si>
+  <si>
+    <t>EEEEE</t>
+  </si>
+  <si>
+    <t>FFFFF</t>
+  </si>
+  <si>
+    <t>GGGG</t>
   </si>
 </sst>
 </file>
@@ -587,7 +587,7 @@
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>